<commit_message>
Added a data validation output with a sheet for new job profile dates that don't have corresponding activity on the worker changes report and one that has a promo or lateral move on the worker changes but not a new job  profile
</commit_message>
<xml_diff>
--- a/outputs/Internal Fill Rate 2025-01-01 to 2025-01-31.xlsx
+++ b/outputs/Internal Fill Rate 2025-01-01 to 2025-01-31.xlsx
@@ -79,13 +79,13 @@
     <t xml:space="preserve">Corp Legal</t>
   </si>
   <si>
+    <t xml:space="preserve">Finance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IPS Industrial Components Division</t>
+  </si>
+  <si>
     <t xml:space="preserve">Corp Sourcing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Finance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IPS Industrial Components Division</t>
   </si>
   <si>
     <t xml:space="preserve">PES APAC</t>
@@ -1464,8 +1464,8 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="A1:R109" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:R109"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="A1:R108" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:R108"/>
   <tableColumns count="18">
     <tableColumn id="1" name="employee_id"/>
     <tableColumn id="2" name="worker"/>
@@ -1788,13 +1788,13 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B2" t="n">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C2" t="n">
-        <v>0.53</v>
+        <v>0.52</v>
       </c>
     </row>
   </sheetData>
@@ -1875,13 +1875,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D5" t="n">
-        <v>0.38</v>
+        <v>0.33</v>
       </c>
     </row>
   </sheetData>
@@ -2124,7 +2124,7 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B14" t="s">
         <v>21</v>
@@ -2141,19 +2141,19 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B15" t="s">
         <v>22</v>
       </c>
       <c r="C15" t="n">
+        <v>1</v>
+      </c>
+      <c r="D15" t="n">
         <v>2</v>
       </c>
-      <c r="D15" t="n">
-        <v>3</v>
-      </c>
       <c r="E15" t="n">
-        <v>0.67</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="16">
@@ -2451,39 +2451,39 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="D8" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E8" t="n">
         <v>3</v>
       </c>
       <c r="F8" t="n">
-        <v>0.67</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D9" t="n">
         <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F9" t="n">
         <v>0</v>
@@ -2494,19 +2494,19 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C10" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10" t="n">
         <v>2</v>
       </c>
       <c r="F10" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="11">
@@ -2517,36 +2517,36 @@
         <v>16</v>
       </c>
       <c r="C11" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D11" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E11" t="n">
         <v>2</v>
       </c>
       <c r="F11" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C12" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="D12" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E12" t="n">
         <v>2</v>
       </c>
       <c r="F12" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="13">
@@ -2554,7 +2554,7 @@
         <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C13" t="s">
         <v>32</v>
@@ -2654,7 +2654,7 @@
         <v>4</v>
       </c>
       <c r="B18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C18" t="s">
         <v>32</v>
@@ -3014,7 +3014,7 @@
         <v>7</v>
       </c>
       <c r="B36" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C36" t="s">
         <v>61</v>
@@ -3034,7 +3034,7 @@
         <v>7</v>
       </c>
       <c r="B37" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C37" t="s">
         <v>60</v>
@@ -3054,7 +3054,7 @@
         <v>7</v>
       </c>
       <c r="B38" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C38" t="s">
         <v>62</v>
@@ -3174,7 +3174,7 @@
         <v>4</v>
       </c>
       <c r="B44" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C44" t="s">
         <v>67</v>
@@ -3724,19 +3724,19 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C9" t="n">
+        <v>2</v>
+      </c>
+      <c r="D9" t="n">
         <v>3</v>
       </c>
-      <c r="D9" t="n">
-        <v>4</v>
-      </c>
       <c r="E9" t="n">
-        <v>0.75</v>
+        <v>0.67</v>
       </c>
     </row>
     <row r="10">
@@ -3744,33 +3744,33 @@
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C10" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D10" t="n">
         <v>3</v>
       </c>
       <c r="E10" t="n">
-        <v>0.67</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C11" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D11" t="n">
         <v>3</v>
       </c>
       <c r="E11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -3778,16 +3778,16 @@
         <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C12" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D12" t="n">
         <v>3</v>
       </c>
       <c r="E12" t="n">
-        <v>0</v>
+        <v>0.67</v>
       </c>
     </row>
     <row r="13">
@@ -4470,7 +4470,7 @@
         <v>7</v>
       </c>
       <c r="G12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H12" t="s">
         <v>61</v>
@@ -4638,7 +4638,7 @@
         <v>4</v>
       </c>
       <c r="G15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H15" t="s">
         <v>67</v>
@@ -5224,7 +5224,7 @@
         <v>7</v>
       </c>
       <c r="G27" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H27" t="s">
         <v>60</v>
@@ -7114,7 +7114,7 @@
         <v>7</v>
       </c>
       <c r="G66" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H66" t="s">
         <v>62</v>
@@ -7278,7 +7278,7 @@
         <v>7</v>
       </c>
       <c r="G69" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H69" t="s">
         <v>32</v>
@@ -7316,13 +7316,13 @@
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
       <c r="B70" t="s">
-        <v>332</v>
+        <v>336</v>
       </c>
       <c r="C70" s="1" t="n">
-        <v>44816</v>
+        <v>44866</v>
       </c>
       <c r="D70" s="1" t="n">
         <v>45670</v>
@@ -7334,49 +7334,49 @@
         <v>7</v>
       </c>
       <c r="G70" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H70" t="s">
         <v>32</v>
       </c>
       <c r="I70" t="s">
-        <v>118</v>
+        <v>337</v>
       </c>
       <c r="J70" s="1" t="n">
         <v>45670</v>
       </c>
       <c r="K70" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="L70" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="M70" t="s">
-        <v>333</v>
+        <v>338</v>
       </c>
       <c r="N70" t="s">
-        <v>148</v>
+        <v>313</v>
       </c>
       <c r="O70" t="s">
-        <v>149</v>
+        <v>177</v>
       </c>
       <c r="P70" t="s">
-        <v>333</v>
+        <v>339</v>
       </c>
       <c r="Q70" t="s">
-        <v>148</v>
+        <v>337</v>
       </c>
       <c r="R70"/>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>335</v>
+        <v>340</v>
       </c>
       <c r="B71" t="s">
-        <v>336</v>
+        <v>341</v>
       </c>
       <c r="C71" s="1" t="n">
-        <v>44866</v>
+        <v>45047</v>
       </c>
       <c r="D71" s="1" t="n">
         <v>45670</v>
@@ -7385,16 +7385,16 @@
         <v>104</v>
       </c>
       <c r="F71" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G71" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="H71" t="s">
         <v>32</v>
       </c>
       <c r="I71" t="s">
-        <v>337</v>
+        <v>132</v>
       </c>
       <c r="J71" s="1" t="n">
         <v>45670</v>
@@ -7406,31 +7406,33 @@
         <v>107</v>
       </c>
       <c r="M71" t="s">
-        <v>338</v>
+        <v>342</v>
       </c>
       <c r="N71" t="s">
-        <v>313</v>
+        <v>148</v>
       </c>
       <c r="O71" t="s">
-        <v>177</v>
+        <v>149</v>
       </c>
       <c r="P71" t="s">
-        <v>339</v>
+        <v>343</v>
       </c>
       <c r="Q71" t="s">
-        <v>337</v>
-      </c>
-      <c r="R71"/>
+        <v>132</v>
+      </c>
+      <c r="R71" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>340</v>
+        <v>344</v>
       </c>
       <c r="B72" t="s">
-        <v>341</v>
+        <v>345</v>
       </c>
       <c r="C72" s="1" t="n">
-        <v>45047</v>
+        <v>42961</v>
       </c>
       <c r="D72" s="1" t="n">
         <v>45670</v>
@@ -7439,54 +7441,36 @@
         <v>104</v>
       </c>
       <c r="F72" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G72" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="H72" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="I72" t="s">
         <v>132</v>
       </c>
-      <c r="J72" s="1" t="n">
-        <v>45670</v>
-      </c>
-      <c r="K72" t="s">
-        <v>106</v>
-      </c>
-      <c r="L72" t="s">
-        <v>107</v>
-      </c>
-      <c r="M72" t="s">
-        <v>342</v>
-      </c>
-      <c r="N72" t="s">
-        <v>148</v>
-      </c>
-      <c r="O72" t="s">
-        <v>149</v>
-      </c>
-      <c r="P72" t="s">
-        <v>343</v>
-      </c>
-      <c r="Q72" t="s">
-        <v>132</v>
-      </c>
-      <c r="R72" t="s">
-        <v>119</v>
-      </c>
+      <c r="J72" s="1"/>
+      <c r="K72"/>
+      <c r="L72"/>
+      <c r="M72"/>
+      <c r="N72"/>
+      <c r="O72"/>
+      <c r="P72"/>
+      <c r="Q72"/>
+      <c r="R72"/>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="B73" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="C73" s="1" t="n">
-        <v>42961</v>
+        <v>45152</v>
       </c>
       <c r="D73" s="1" t="n">
         <v>45670</v>
@@ -7498,75 +7482,87 @@
         <v>6</v>
       </c>
       <c r="G73" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H73" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="I73" t="s">
-        <v>132</v>
-      </c>
-      <c r="J73" s="1"/>
-      <c r="K73"/>
-      <c r="L73"/>
-      <c r="M73"/>
-      <c r="N73"/>
-      <c r="O73"/>
-      <c r="P73"/>
-      <c r="Q73"/>
-      <c r="R73"/>
+        <v>105</v>
+      </c>
+      <c r="J73" s="1" t="n">
+        <v>45670</v>
+      </c>
+      <c r="K73" t="s">
+        <v>106</v>
+      </c>
+      <c r="L73" t="s">
+        <v>107</v>
+      </c>
+      <c r="M73" t="s">
+        <v>348</v>
+      </c>
+      <c r="N73" t="s">
+        <v>114</v>
+      </c>
+      <c r="O73" t="s">
+        <v>149</v>
+      </c>
+      <c r="P73" t="s">
+        <v>182</v>
+      </c>
+      <c r="Q73" t="s">
+        <v>105</v>
+      </c>
+      <c r="R73" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="B74" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="C74" s="1" t="n">
-        <v>45152</v>
+        <v>45670</v>
       </c>
       <c r="D74" s="1" t="n">
         <v>45670</v>
       </c>
       <c r="E74" t="s">
-        <v>104</v>
+        <v>204</v>
       </c>
       <c r="F74" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G74" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H74" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="I74" t="s">
-        <v>105</v>
+        <v>118</v>
       </c>
       <c r="J74" s="1" t="n">
         <v>45670</v>
       </c>
       <c r="K74" t="s">
-        <v>106</v>
+        <v>205</v>
       </c>
       <c r="L74" t="s">
-        <v>107</v>
-      </c>
-      <c r="M74" t="s">
-        <v>348</v>
-      </c>
-      <c r="N74" t="s">
-        <v>114</v>
-      </c>
-      <c r="O74" t="s">
-        <v>149</v>
-      </c>
+        <v>206</v>
+      </c>
+      <c r="M74"/>
+      <c r="N74"/>
+      <c r="O74"/>
       <c r="P74" t="s">
-        <v>182</v>
+        <v>319</v>
       </c>
       <c r="Q74" t="s">
-        <v>105</v>
+        <v>118</v>
       </c>
       <c r="R74" t="s">
         <v>121</v>
@@ -7574,10 +7570,10 @@
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="B75" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="C75" s="1" t="n">
         <v>45670</v>
@@ -7592,13 +7588,13 @@
         <v>4</v>
       </c>
       <c r="G75" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="H75" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="I75" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="J75" s="1" t="n">
         <v>45670</v>
@@ -7613,10 +7609,10 @@
       <c r="N75"/>
       <c r="O75"/>
       <c r="P75" t="s">
-        <v>319</v>
+        <v>353</v>
       </c>
       <c r="Q75" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="R75" t="s">
         <v>121</v>
@@ -7624,10 +7620,10 @@
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="B76" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="C76" s="1" t="n">
         <v>45670</v>
@@ -7639,16 +7635,16 @@
         <v>204</v>
       </c>
       <c r="F76" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="G76" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="H76" t="s">
         <v>32</v>
       </c>
       <c r="I76" t="s">
-        <v>114</v>
+        <v>313</v>
       </c>
       <c r="J76" s="1" t="n">
         <v>45670</v>
@@ -7663,21 +7659,21 @@
       <c r="N76"/>
       <c r="O76"/>
       <c r="P76" t="s">
-        <v>353</v>
+        <v>338</v>
       </c>
       <c r="Q76" t="s">
-        <v>114</v>
+        <v>313</v>
       </c>
       <c r="R76" t="s">
-        <v>121</v>
+        <v>177</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="B77" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="C77" s="1" t="n">
         <v>45670</v>
@@ -7689,16 +7685,16 @@
         <v>204</v>
       </c>
       <c r="F77" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G77" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="H77" t="s">
         <v>32</v>
       </c>
       <c r="I77" t="s">
-        <v>313</v>
+        <v>114</v>
       </c>
       <c r="J77" s="1" t="n">
         <v>45670</v>
@@ -7713,21 +7709,21 @@
       <c r="N77"/>
       <c r="O77"/>
       <c r="P77" t="s">
-        <v>338</v>
+        <v>327</v>
       </c>
       <c r="Q77" t="s">
-        <v>313</v>
+        <v>114</v>
       </c>
       <c r="R77" t="s">
-        <v>177</v>
+        <v>121</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="B78" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="C78" s="1" t="n">
         <v>45670</v>
@@ -7763,7 +7759,7 @@
       <c r="N78"/>
       <c r="O78"/>
       <c r="P78" t="s">
-        <v>327</v>
+        <v>360</v>
       </c>
       <c r="Q78" t="s">
         <v>114</v>
@@ -7774,10 +7770,10 @@
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>358</v>
+        <v>361</v>
       </c>
       <c r="B79" t="s">
-        <v>359</v>
+        <v>362</v>
       </c>
       <c r="C79" s="1" t="n">
         <v>45670</v>
@@ -7789,16 +7785,16 @@
         <v>204</v>
       </c>
       <c r="F79" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G79" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="H79" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I79" t="s">
-        <v>114</v>
+        <v>174</v>
       </c>
       <c r="J79" s="1" t="n">
         <v>45670</v>
@@ -7813,21 +7809,21 @@
       <c r="N79"/>
       <c r="O79"/>
       <c r="P79" t="s">
-        <v>360</v>
+        <v>254</v>
       </c>
       <c r="Q79" t="s">
-        <v>114</v>
+        <v>174</v>
       </c>
       <c r="R79" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="B80" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="C80" s="1" t="n">
         <v>45670</v>
@@ -7839,16 +7835,16 @@
         <v>204</v>
       </c>
       <c r="F80" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G80" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H80" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I80" t="s">
-        <v>174</v>
+        <v>132</v>
       </c>
       <c r="J80" s="1" t="n">
         <v>45670</v>
@@ -7863,21 +7859,21 @@
       <c r="N80"/>
       <c r="O80"/>
       <c r="P80" t="s">
-        <v>254</v>
+        <v>365</v>
       </c>
       <c r="Q80" t="s">
-        <v>174</v>
+        <v>132</v>
       </c>
       <c r="R80" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>363</v>
+        <v>366</v>
       </c>
       <c r="B81" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
       <c r="C81" s="1" t="n">
         <v>45670</v>
@@ -7889,16 +7885,16 @@
         <v>204</v>
       </c>
       <c r="F81" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G81" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H81" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="I81" t="s">
-        <v>132</v>
+        <v>114</v>
       </c>
       <c r="J81" s="1" t="n">
         <v>45670</v>
@@ -7913,21 +7909,21 @@
       <c r="N81"/>
       <c r="O81"/>
       <c r="P81" t="s">
-        <v>365</v>
+        <v>158</v>
       </c>
       <c r="Q81" t="s">
-        <v>132</v>
+        <v>114</v>
       </c>
       <c r="R81" t="s">
-        <v>119</v>
+        <v>149</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="B82" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="C82" s="1" t="n">
         <v>45670</v>
@@ -7963,7 +7959,7 @@
       <c r="N82"/>
       <c r="O82"/>
       <c r="P82" t="s">
-        <v>158</v>
+        <v>370</v>
       </c>
       <c r="Q82" t="s">
         <v>114</v>
@@ -7974,10 +7970,10 @@
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
       <c r="B83" t="s">
-        <v>369</v>
+        <v>372</v>
       </c>
       <c r="C83" s="1" t="n">
         <v>45670</v>
@@ -7989,16 +7985,16 @@
         <v>204</v>
       </c>
       <c r="F83" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G83" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="H83" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I83" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="J83" s="1" t="n">
         <v>45670</v>
@@ -8013,21 +8009,21 @@
       <c r="N83"/>
       <c r="O83"/>
       <c r="P83" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="Q83" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="R83" t="s">
-        <v>149</v>
+        <v>121</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
       <c r="B84" t="s">
-        <v>372</v>
+        <v>375</v>
       </c>
       <c r="C84" s="1" t="n">
         <v>45670</v>
@@ -8039,16 +8035,16 @@
         <v>204</v>
       </c>
       <c r="F84" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G84" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="H84" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="I84" t="s">
-        <v>118</v>
+        <v>376</v>
       </c>
       <c r="J84" s="1" t="n">
         <v>45670</v>
@@ -8063,21 +8059,21 @@
       <c r="N84"/>
       <c r="O84"/>
       <c r="P84" t="s">
-        <v>373</v>
+        <v>377</v>
       </c>
       <c r="Q84" t="s">
-        <v>118</v>
+        <v>376</v>
       </c>
       <c r="R84" t="s">
-        <v>121</v>
+        <v>378</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="s">
-        <v>374</v>
+        <v>379</v>
       </c>
       <c r="B85" t="s">
-        <v>375</v>
+        <v>380</v>
       </c>
       <c r="C85" s="1" t="n">
         <v>45670</v>
@@ -8092,13 +8088,13 @@
         <v>4</v>
       </c>
       <c r="G85" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="H85" t="s">
-        <v>32</v>
+        <v>65</v>
       </c>
       <c r="I85" t="s">
-        <v>376</v>
+        <v>118</v>
       </c>
       <c r="J85" s="1" t="n">
         <v>45670</v>
@@ -8113,21 +8109,21 @@
       <c r="N85"/>
       <c r="O85"/>
       <c r="P85" t="s">
-        <v>377</v>
+        <v>381</v>
       </c>
       <c r="Q85" t="s">
-        <v>376</v>
+        <v>118</v>
       </c>
       <c r="R85" t="s">
-        <v>378</v>
+        <v>121</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="s">
-        <v>379</v>
+        <v>382</v>
       </c>
       <c r="B86" t="s">
-        <v>380</v>
+        <v>383</v>
       </c>
       <c r="C86" s="1" t="n">
         <v>45670</v>
@@ -8139,16 +8135,16 @@
         <v>204</v>
       </c>
       <c r="F86" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G86" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="H86" t="s">
-        <v>65</v>
+        <v>35</v>
       </c>
       <c r="I86" t="s">
-        <v>118</v>
+        <v>313</v>
       </c>
       <c r="J86" s="1" t="n">
         <v>45670</v>
@@ -8163,21 +8159,21 @@
       <c r="N86"/>
       <c r="O86"/>
       <c r="P86" t="s">
-        <v>381</v>
+        <v>384</v>
       </c>
       <c r="Q86" t="s">
-        <v>118</v>
+        <v>313</v>
       </c>
       <c r="R86" t="s">
-        <v>121</v>
+        <v>177</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="s">
-        <v>382</v>
+        <v>385</v>
       </c>
       <c r="B87" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="C87" s="1" t="n">
         <v>45670</v>
@@ -8195,10 +8191,10 @@
         <v>10</v>
       </c>
       <c r="H87" t="s">
-        <v>35</v>
+        <v>78</v>
       </c>
       <c r="I87" t="s">
-        <v>313</v>
+        <v>132</v>
       </c>
       <c r="J87" s="1" t="n">
         <v>45670</v>
@@ -8213,27 +8209,27 @@
       <c r="N87"/>
       <c r="O87"/>
       <c r="P87" t="s">
-        <v>384</v>
+        <v>387</v>
       </c>
       <c r="Q87" t="s">
-        <v>313</v>
+        <v>132</v>
       </c>
       <c r="R87" t="s">
-        <v>177</v>
+        <v>127</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="s">
-        <v>385</v>
+        <v>388</v>
       </c>
       <c r="B88" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
       <c r="C88" s="1" t="n">
-        <v>45670</v>
+        <v>45672</v>
       </c>
       <c r="D88" s="1" t="n">
-        <v>45670</v>
+        <v>45672</v>
       </c>
       <c r="E88" t="s">
         <v>204</v>
@@ -8242,16 +8238,16 @@
         <v>5</v>
       </c>
       <c r="G88" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="H88" t="s">
-        <v>78</v>
+        <v>32</v>
       </c>
       <c r="I88" t="s">
-        <v>132</v>
+        <v>174</v>
       </c>
       <c r="J88" s="1" t="n">
-        <v>45670</v>
+        <v>45672</v>
       </c>
       <c r="K88" t="s">
         <v>205</v>
@@ -8263,10 +8259,10 @@
       <c r="N88"/>
       <c r="O88"/>
       <c r="P88" t="s">
-        <v>387</v>
+        <v>390</v>
       </c>
       <c r="Q88" t="s">
-        <v>132</v>
+        <v>174</v>
       </c>
       <c r="R88" t="s">
         <v>127</v>
@@ -8274,116 +8270,116 @@
     </row>
     <row r="89">
       <c r="A89" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
       <c r="B89" t="s">
-        <v>389</v>
+        <v>392</v>
       </c>
       <c r="C89" s="1" t="n">
-        <v>45672</v>
+        <v>42508</v>
       </c>
       <c r="D89" s="1" t="n">
-        <v>45672</v>
+        <v>45677</v>
       </c>
       <c r="E89" t="s">
-        <v>204</v>
+        <v>104</v>
       </c>
       <c r="F89" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G89" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="H89" t="s">
         <v>32</v>
       </c>
       <c r="I89" t="s">
+        <v>118</v>
+      </c>
+      <c r="J89" s="1" t="n">
+        <v>45677</v>
+      </c>
+      <c r="K89" t="s">
+        <v>115</v>
+      </c>
+      <c r="L89" t="s">
+        <v>393</v>
+      </c>
+      <c r="M89" t="s">
+        <v>254</v>
+      </c>
+      <c r="N89" t="s">
         <v>174</v>
       </c>
-      <c r="J89" s="1" t="n">
-        <v>45672</v>
-      </c>
-      <c r="K89" t="s">
-        <v>205</v>
-      </c>
-      <c r="L89" t="s">
-        <v>206</v>
-      </c>
-      <c r="M89"/>
-      <c r="N89"/>
-      <c r="O89"/>
+      <c r="O89" t="s">
+        <v>127</v>
+      </c>
       <c r="P89" t="s">
-        <v>390</v>
+        <v>394</v>
       </c>
       <c r="Q89" t="s">
-        <v>174</v>
+        <v>118</v>
       </c>
       <c r="R89" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="s">
-        <v>391</v>
+        <v>395</v>
       </c>
       <c r="B90" t="s">
-        <v>392</v>
+        <v>396</v>
       </c>
       <c r="C90" s="1" t="n">
-        <v>42508</v>
+        <v>45677</v>
       </c>
       <c r="D90" s="1" t="n">
         <v>45677</v>
       </c>
       <c r="E90" t="s">
-        <v>104</v>
+        <v>204</v>
       </c>
       <c r="F90" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G90" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="H90" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="I90" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
       <c r="J90" s="1" t="n">
         <v>45677</v>
       </c>
       <c r="K90" t="s">
-        <v>115</v>
+        <v>205</v>
       </c>
       <c r="L90" t="s">
-        <v>393</v>
-      </c>
-      <c r="M90" t="s">
-        <v>254</v>
-      </c>
-      <c r="N90" t="s">
-        <v>174</v>
-      </c>
-      <c r="O90" t="s">
-        <v>127</v>
-      </c>
+        <v>206</v>
+      </c>
+      <c r="M90"/>
+      <c r="N90"/>
+      <c r="O90"/>
       <c r="P90" t="s">
-        <v>394</v>
+        <v>110</v>
       </c>
       <c r="Q90" t="s">
-        <v>118</v>
+        <v>105</v>
       </c>
       <c r="R90" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="B91" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="C91" s="1" t="n">
         <v>45677</v>
@@ -8395,16 +8391,16 @@
         <v>204</v>
       </c>
       <c r="F91" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G91" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="H91" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="I91" t="s">
-        <v>105</v>
+        <v>132</v>
       </c>
       <c r="J91" s="1" t="n">
         <v>45677</v>
@@ -8419,21 +8415,21 @@
       <c r="N91"/>
       <c r="O91"/>
       <c r="P91" t="s">
-        <v>110</v>
+        <v>399</v>
       </c>
       <c r="Q91" t="s">
-        <v>105</v>
+        <v>132</v>
       </c>
       <c r="R91" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="s">
-        <v>397</v>
+        <v>400</v>
       </c>
       <c r="B92" t="s">
-        <v>398</v>
+        <v>401</v>
       </c>
       <c r="C92" s="1" t="n">
         <v>45677</v>
@@ -8448,13 +8444,13 @@
         <v>7</v>
       </c>
       <c r="G92" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="H92" t="s">
-        <v>59</v>
+        <v>32</v>
       </c>
       <c r="I92" t="s">
-        <v>132</v>
+        <v>114</v>
       </c>
       <c r="J92" s="1" t="n">
         <v>45677</v>
@@ -8469,21 +8465,21 @@
       <c r="N92"/>
       <c r="O92"/>
       <c r="P92" t="s">
-        <v>399</v>
+        <v>327</v>
       </c>
       <c r="Q92" t="s">
-        <v>132</v>
+        <v>114</v>
       </c>
       <c r="R92" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="B93" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="C93" s="1" t="n">
         <v>45677</v>
@@ -8495,16 +8491,16 @@
         <v>204</v>
       </c>
       <c r="F93" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G93" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="H93" t="s">
-        <v>32</v>
+        <v>68</v>
       </c>
       <c r="I93" t="s">
-        <v>114</v>
+        <v>161</v>
       </c>
       <c r="J93" s="1" t="n">
         <v>45677</v>
@@ -8519,21 +8515,21 @@
       <c r="N93"/>
       <c r="O93"/>
       <c r="P93" t="s">
-        <v>327</v>
+        <v>163</v>
       </c>
       <c r="Q93" t="s">
-        <v>114</v>
+        <v>161</v>
       </c>
       <c r="R93" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="B94" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="C94" s="1" t="n">
         <v>45677</v>
@@ -8551,10 +8547,10 @@
         <v>9</v>
       </c>
       <c r="H94" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="I94" t="s">
-        <v>161</v>
+        <v>114</v>
       </c>
       <c r="J94" s="1" t="n">
         <v>45677</v>
@@ -8569,21 +8565,21 @@
       <c r="N94"/>
       <c r="O94"/>
       <c r="P94" t="s">
-        <v>163</v>
+        <v>125</v>
       </c>
       <c r="Q94" t="s">
-        <v>161</v>
+        <v>114</v>
       </c>
       <c r="R94" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="B95" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="C95" s="1" t="n">
         <v>45677</v>
@@ -8595,16 +8591,16 @@
         <v>204</v>
       </c>
       <c r="F95" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G95" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="H95" t="s">
-        <v>73</v>
+        <v>49</v>
       </c>
       <c r="I95" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="J95" s="1" t="n">
         <v>45677</v>
@@ -8619,21 +8615,21 @@
       <c r="N95"/>
       <c r="O95"/>
       <c r="P95" t="s">
-        <v>125</v>
+        <v>408</v>
       </c>
       <c r="Q95" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="R95" t="s">
-        <v>121</v>
+        <v>149</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="s">
-        <v>406</v>
+        <v>409</v>
       </c>
       <c r="B96" t="s">
-        <v>407</v>
+        <v>410</v>
       </c>
       <c r="C96" s="1" t="n">
         <v>45677</v>
@@ -8645,13 +8641,13 @@
         <v>204</v>
       </c>
       <c r="F96" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G96" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H96" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="I96" t="s">
         <v>105</v>
@@ -8669,7 +8665,7 @@
       <c r="N96"/>
       <c r="O96"/>
       <c r="P96" t="s">
-        <v>408</v>
+        <v>170</v>
       </c>
       <c r="Q96" t="s">
         <v>105</v>
@@ -8680,10 +8676,10 @@
     </row>
     <row r="97">
       <c r="A97" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="B97" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="C97" s="1" t="n">
         <v>45677</v>
@@ -8704,7 +8700,7 @@
         <v>43</v>
       </c>
       <c r="I97" t="s">
-        <v>105</v>
+        <v>118</v>
       </c>
       <c r="J97" s="1" t="n">
         <v>45677</v>
@@ -8719,80 +8715,82 @@
       <c r="N97"/>
       <c r="O97"/>
       <c r="P97" t="s">
-        <v>170</v>
+        <v>117</v>
       </c>
       <c r="Q97" t="s">
-        <v>105</v>
+        <v>118</v>
       </c>
       <c r="R97" t="s">
-        <v>149</v>
+        <v>119</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="B98" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="C98" s="1" t="n">
-        <v>45677</v>
+        <v>45679</v>
       </c>
       <c r="D98" s="1" t="n">
-        <v>45677</v>
+        <v>45679</v>
       </c>
       <c r="E98" t="s">
         <v>204</v>
       </c>
       <c r="F98" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G98" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H98" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="I98" t="s">
         <v>118</v>
       </c>
       <c r="J98" s="1" t="n">
-        <v>45677</v>
+        <v>45679</v>
       </c>
       <c r="K98" t="s">
         <v>205</v>
       </c>
       <c r="L98" t="s">
-        <v>206</v>
+        <v>235</v>
       </c>
       <c r="M98"/>
       <c r="N98"/>
-      <c r="O98"/>
+      <c r="O98" t="s">
+        <v>121</v>
+      </c>
       <c r="P98" t="s">
-        <v>117</v>
+        <v>381</v>
       </c>
       <c r="Q98" t="s">
         <v>118</v>
       </c>
       <c r="R98" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="B99" t="s">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="C99" s="1" t="n">
-        <v>45679</v>
+        <v>44608</v>
       </c>
       <c r="D99" s="1" t="n">
-        <v>45679</v>
+        <v>45684</v>
       </c>
       <c r="E99" t="s">
-        <v>204</v>
+        <v>104</v>
       </c>
       <c r="F99" t="s">
         <v>6</v>
@@ -8804,41 +8802,27 @@
         <v>36</v>
       </c>
       <c r="I99" t="s">
-        <v>118</v>
-      </c>
-      <c r="J99" s="1" t="n">
-        <v>45679</v>
-      </c>
-      <c r="K99" t="s">
-        <v>205</v>
-      </c>
-      <c r="L99" t="s">
-        <v>235</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="J99" s="1"/>
+      <c r="K99"/>
+      <c r="L99"/>
       <c r="M99"/>
       <c r="N99"/>
-      <c r="O99" t="s">
-        <v>121</v>
-      </c>
-      <c r="P99" t="s">
-        <v>381</v>
-      </c>
-      <c r="Q99" t="s">
-        <v>118</v>
-      </c>
-      <c r="R99" t="s">
-        <v>121</v>
-      </c>
+      <c r="O99"/>
+      <c r="P99"/>
+      <c r="Q99"/>
+      <c r="R99"/>
     </row>
     <row r="100">
       <c r="A100" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="B100" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="C100" s="1" t="n">
-        <v>44608</v>
+        <v>38887</v>
       </c>
       <c r="D100" s="1" t="n">
         <v>45684</v>
@@ -8847,89 +8831,101 @@
         <v>104</v>
       </c>
       <c r="F100" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G100" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="H100" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="I100" t="s">
-        <v>105</v>
-      </c>
-      <c r="J100" s="1"/>
-      <c r="K100"/>
-      <c r="L100"/>
-      <c r="M100"/>
-      <c r="N100"/>
-      <c r="O100"/>
-      <c r="P100"/>
-      <c r="Q100"/>
-      <c r="R100"/>
+        <v>132</v>
+      </c>
+      <c r="J100" s="1" t="n">
+        <v>45684</v>
+      </c>
+      <c r="K100" t="s">
+        <v>106</v>
+      </c>
+      <c r="L100" t="s">
+        <v>107</v>
+      </c>
+      <c r="M100" t="s">
+        <v>419</v>
+      </c>
+      <c r="N100" t="s">
+        <v>118</v>
+      </c>
+      <c r="O100" t="s">
+        <v>149</v>
+      </c>
+      <c r="P100" t="s">
+        <v>420</v>
+      </c>
+      <c r="Q100" t="s">
+        <v>132</v>
+      </c>
+      <c r="R100" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="s">
-        <v>417</v>
+        <v>421</v>
       </c>
       <c r="B101" t="s">
-        <v>418</v>
+        <v>422</v>
       </c>
       <c r="C101" s="1" t="n">
-        <v>38887</v>
+        <v>45684</v>
       </c>
       <c r="D101" s="1" t="n">
         <v>45684</v>
       </c>
       <c r="E101" t="s">
-        <v>104</v>
+        <v>204</v>
       </c>
       <c r="F101" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G101" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="H101" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="I101" t="s">
-        <v>132</v>
+        <v>105</v>
       </c>
       <c r="J101" s="1" t="n">
         <v>45684</v>
       </c>
       <c r="K101" t="s">
-        <v>106</v>
+        <v>205</v>
       </c>
       <c r="L101" t="s">
-        <v>107</v>
-      </c>
-      <c r="M101" t="s">
-        <v>419</v>
-      </c>
-      <c r="N101" t="s">
-        <v>118</v>
-      </c>
-      <c r="O101" t="s">
+        <v>206</v>
+      </c>
+      <c r="M101"/>
+      <c r="N101"/>
+      <c r="O101"/>
+      <c r="P101" t="s">
+        <v>207</v>
+      </c>
+      <c r="Q101" t="s">
+        <v>105</v>
+      </c>
+      <c r="R101" t="s">
         <v>149</v>
-      </c>
-      <c r="P101" t="s">
-        <v>420</v>
-      </c>
-      <c r="Q101" t="s">
-        <v>132</v>
-      </c>
-      <c r="R101" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="B102" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
       <c r="C102" s="1" t="n">
         <v>45684</v>
@@ -8944,13 +8940,13 @@
         <v>6</v>
       </c>
       <c r="G102" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="H102" t="s">
-        <v>38</v>
+        <v>57</v>
       </c>
       <c r="I102" t="s">
-        <v>105</v>
+        <v>118</v>
       </c>
       <c r="J102" s="1" t="n">
         <v>45684</v>
@@ -8965,21 +8961,21 @@
       <c r="N102"/>
       <c r="O102"/>
       <c r="P102" t="s">
-        <v>207</v>
+        <v>167</v>
       </c>
       <c r="Q102" t="s">
-        <v>105</v>
+        <v>118</v>
       </c>
       <c r="R102" t="s">
-        <v>149</v>
+        <v>121</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="B103" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="C103" s="1" t="n">
         <v>45684</v>
@@ -8991,16 +8987,16 @@
         <v>204</v>
       </c>
       <c r="F103" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G103" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="H103" t="s">
-        <v>57</v>
+        <v>32</v>
       </c>
       <c r="I103" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="J103" s="1" t="n">
         <v>45684</v>
@@ -9015,21 +9011,21 @@
       <c r="N103"/>
       <c r="O103"/>
       <c r="P103" t="s">
-        <v>167</v>
+        <v>427</v>
       </c>
       <c r="Q103" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="R103" t="s">
-        <v>121</v>
+        <v>149</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="s">
-        <v>425</v>
+        <v>428</v>
       </c>
       <c r="B104" t="s">
-        <v>426</v>
+        <v>429</v>
       </c>
       <c r="C104" s="1" t="n">
         <v>45684</v>
@@ -9041,16 +9037,16 @@
         <v>204</v>
       </c>
       <c r="F104" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G104" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H104" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I104" t="s">
-        <v>114</v>
+        <v>174</v>
       </c>
       <c r="J104" s="1" t="n">
         <v>45684</v>
@@ -9065,21 +9061,21 @@
       <c r="N104"/>
       <c r="O104"/>
       <c r="P104" t="s">
-        <v>427</v>
+        <v>430</v>
       </c>
       <c r="Q104" t="s">
-        <v>114</v>
+        <v>174</v>
       </c>
       <c r="R104" t="s">
-        <v>149</v>
+        <v>177</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="s">
-        <v>428</v>
+        <v>431</v>
       </c>
       <c r="B105" t="s">
-        <v>429</v>
+        <v>432</v>
       </c>
       <c r="C105" s="1" t="n">
         <v>45684</v>
@@ -9097,10 +9093,10 @@
         <v>10</v>
       </c>
       <c r="H105" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="I105" t="s">
-        <v>174</v>
+        <v>114</v>
       </c>
       <c r="J105" s="1" t="n">
         <v>45684</v>
@@ -9115,21 +9111,21 @@
       <c r="N105"/>
       <c r="O105"/>
       <c r="P105" t="s">
-        <v>430</v>
+        <v>433</v>
       </c>
       <c r="Q105" t="s">
-        <v>174</v>
+        <v>114</v>
       </c>
       <c r="R105" t="s">
-        <v>177</v>
+        <v>149</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="s">
-        <v>431</v>
+        <v>434</v>
       </c>
       <c r="B106" t="s">
-        <v>432</v>
+        <v>435</v>
       </c>
       <c r="C106" s="1" t="n">
         <v>45684</v>
@@ -9147,10 +9143,10 @@
         <v>10</v>
       </c>
       <c r="H106" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="I106" t="s">
-        <v>114</v>
+        <v>132</v>
       </c>
       <c r="J106" s="1" t="n">
         <v>45684</v>
@@ -9165,21 +9161,21 @@
       <c r="N106"/>
       <c r="O106"/>
       <c r="P106" t="s">
-        <v>433</v>
+        <v>436</v>
       </c>
       <c r="Q106" t="s">
-        <v>114</v>
+        <v>132</v>
       </c>
       <c r="R106" t="s">
-        <v>149</v>
+        <v>121</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="s">
-        <v>434</v>
+        <v>437</v>
       </c>
       <c r="B107" t="s">
-        <v>435</v>
+        <v>438</v>
       </c>
       <c r="C107" s="1" t="n">
         <v>45684</v>
@@ -9191,16 +9187,16 @@
         <v>204</v>
       </c>
       <c r="F107" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G107" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H107" t="s">
-        <v>35</v>
+        <v>72</v>
       </c>
       <c r="I107" t="s">
-        <v>132</v>
+        <v>161</v>
       </c>
       <c r="J107" s="1" t="n">
         <v>45684</v>
@@ -9215,102 +9211,52 @@
       <c r="N107"/>
       <c r="O107"/>
       <c r="P107" t="s">
-        <v>436</v>
+        <v>439</v>
       </c>
       <c r="Q107" t="s">
-        <v>132</v>
+        <v>161</v>
       </c>
       <c r="R107" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="s">
-        <v>437</v>
+        <v>440</v>
       </c>
       <c r="B108" t="s">
-        <v>438</v>
+        <v>441</v>
       </c>
       <c r="C108" s="1" t="n">
-        <v>45684</v>
+        <v>45688</v>
       </c>
       <c r="D108" s="1" t="n">
-        <v>45684</v>
+        <v>45688</v>
       </c>
       <c r="E108" t="s">
         <v>204</v>
       </c>
       <c r="F108" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G108" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="H108" t="s">
-        <v>72</v>
+        <v>39</v>
       </c>
       <c r="I108" t="s">
-        <v>161</v>
-      </c>
-      <c r="J108" s="1" t="n">
-        <v>45684</v>
-      </c>
-      <c r="K108" t="s">
-        <v>205</v>
-      </c>
-      <c r="L108" t="s">
-        <v>206</v>
-      </c>
+        <v>118</v>
+      </c>
+      <c r="J108" s="1"/>
+      <c r="K108"/>
+      <c r="L108"/>
       <c r="M108"/>
       <c r="N108"/>
       <c r="O108"/>
-      <c r="P108" t="s">
-        <v>439</v>
-      </c>
-      <c r="Q108" t="s">
-        <v>161</v>
-      </c>
-      <c r="R108" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="109">
-      <c r="A109" t="s">
-        <v>440</v>
-      </c>
-      <c r="B109" t="s">
-        <v>441</v>
-      </c>
-      <c r="C109" s="1" t="n">
-        <v>45688</v>
-      </c>
-      <c r="D109" s="1" t="n">
-        <v>45688</v>
-      </c>
-      <c r="E109" t="s">
-        <v>204</v>
-      </c>
-      <c r="F109" t="s">
-        <v>6</v>
-      </c>
-      <c r="G109" t="s">
-        <v>16</v>
-      </c>
-      <c r="H109" t="s">
-        <v>39</v>
-      </c>
-      <c r="I109" t="s">
-        <v>118</v>
-      </c>
-      <c r="J109" s="1"/>
-      <c r="K109"/>
-      <c r="L109"/>
-      <c r="M109"/>
-      <c r="N109"/>
-      <c r="O109"/>
-      <c r="P109"/>
-      <c r="Q109"/>
-      <c r="R109"/>
+      <c r="P108"/>
+      <c r="Q108"/>
+      <c r="R108"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>